<commit_message>
First drafts for code to clean NC routine and conditional data.
Code does not include merging of routine and conditional data (will be another script).

Edited NC conditional excel files to run with code.
 Minimal edits were made. Primarily deleted empty sheets and renamed column headers to match code (uppercase vs lowercase, added spaces, etc).
</commit_message>
<xml_diff>
--- a/data/nc/conditional_sampling_ncdmf/datasheets/cond_b8.xlsx
+++ b/data/nc/conditional_sampling_ncdmf/datasheets/cond_b8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/megancarr/Documents/400_data_analytics/shellbase_bal/data/nc/conditional_sampling_ncdmf/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCD4454E-3DC5-8F4B-B8D8-40B28FB11CD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F038DCE-C1E6-F644-BC49-F38895868AC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="1520" windowWidth="25640" windowHeight="12820" xr2:uid="{10307CD1-DA8B-C748-BDD5-2CA138E43A01}"/>
   </bookViews>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>STATION</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
   <si>
     <t>PD1</t>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>NO.</t>
   </si>
 </sst>
 </file>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16506645-F3BB-E348-AB55-E304E6DD11B7}">
   <dimension ref="A1:HD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="GM1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -522,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D1" s="2">
         <v>33983</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="2" spans="1:212" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="3" spans="1:212" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="5"/>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="4" spans="1:212" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4">
         <v>39</v>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="5" spans="1:212" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5"/>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="6" spans="1:212" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="4">
         <v>8</v>
@@ -1916,10 +1916,10 @@
     </row>
     <row r="7" spans="1:212" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="C7" s="5"/>
       <c r="AF7" s="6">
@@ -1986,7 +1986,7 @@
     </row>
     <row r="8" spans="1:212" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4">
         <v>13</v>
@@ -2191,7 +2191,7 @@
         <v>540</v>
       </c>
       <c r="GB8" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="GC8" s="6">
         <v>6.8</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="9" spans="1:212" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="4">
         <v>26</v>
@@ -2477,13 +2477,13 @@
     </row>
     <row r="10" spans="1:212" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="4">
         <v>36</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="11" spans="1:212" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="5"/>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="12" spans="1:212" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="4">
         <v>17</v>
@@ -3372,7 +3372,7 @@
         <v>49</v>
       </c>
       <c r="GB12" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="GC12" s="6">
         <v>7.8</v>
@@ -3428,10 +3428,10 @@
     </row>
     <row r="13" spans="1:212" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="C13" s="5"/>
       <c r="AP13" s="6">
@@ -3476,7 +3476,7 @@
         <v>22</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="6">
         <v>49</v>
@@ -3899,7 +3899,7 @@
         <v>110</v>
       </c>
       <c r="GB14" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="GC14" s="6">
         <v>7.8</v>
@@ -3926,7 +3926,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="6">
         <v>11</v>
@@ -4275,7 +4275,7 @@
         <v>33</v>
       </c>
       <c r="GB15" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="GC15" s="6">
         <v>2</v>
@@ -4305,7 +4305,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="6">
         <v>13</v>
@@ -4677,7 +4677,7 @@
         <v>70</v>
       </c>
       <c r="GB16" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="GC16" s="6">
         <v>2</v>
@@ -4707,7 +4707,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="6">
         <v>7.8</v>
@@ -5076,7 +5076,7 @@
         <v>27</v>
       </c>
       <c r="GB17" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="GC17" s="6">
         <v>1.7</v>
@@ -5144,7 +5144,7 @@
     <row r="20" spans="1:197" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="5"/>
       <c r="AF20" s="6">
@@ -5185,7 +5185,7 @@
     <row r="21" spans="1:197" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="5"/>
       <c r="AF21" s="6">
@@ -5246,7 +5246,7 @@
         <v>10</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -5351,7 +5351,7 @@
         <v>41</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="6">
         <v>23</v>
@@ -5667,7 +5667,7 @@
         <v>10</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -5990,7 +5990,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="CS29" s="6"/>
       <c r="CT29" s="6"/>
@@ -6102,7 +6102,7 @@
         <v>46</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="CS30" s="6"/>
       <c r="CT30" s="6"/>
@@ -6357,7 +6357,7 @@
         <v>6</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="FZ36" s="9">
         <v>2</v>

</xml_diff>